<commit_message>
Add updated grammar conversion spreadsheet
</commit_message>
<xml_diff>
--- a/source_language_spec/Grammar_Conversion.xlsx
+++ b/source_language_spec/Grammar_Conversion.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d42660897f176d1e/Documents/Uni/2022/Semester 2/COMP3290/Assessment/Assignment 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A55B4F5E-CA0E-4ACA-B9A2-3FA6FE79AEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="344" documentId="8_{4B6A1E2B-9DE3-4CEB-8A4E-7724E9331625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08EE5BEE-A678-4F03-8B38-AC2B5220AC6A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{CAC1321C-A57E-482A-BF8B-9CDDCA90FB4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAC1321C-A57E-482A-BF8B-9CDDCA90FB4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet2!$B$1:$O$105</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="252">
   <si>
     <t>Node</t>
   </si>
@@ -56,9 +59,6 @@
     <t>Left Recursion</t>
   </si>
   <si>
-    <t>Symbol Table Entry</t>
-  </si>
-  <si>
     <t>NPROG</t>
   </si>
   <si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>CD22, ID done globals started</t>
-  </si>
-  <si>
-    <t>Program Identifier</t>
   </si>
   <si>
     <t>NGLOB</t>
@@ -137,9 +134,6 @@
     <t xml:space="preserve">::= &lt;id&gt; = &lt;expr&gt; </t>
   </si>
   <si>
-    <t>Constant Value</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;types&gt; </t>
   </si>
   <si>
@@ -233,18 +227,12 @@
     <t xml:space="preserve">::= &lt;structid&gt; def &lt;fields&gt; end </t>
   </si>
   <si>
-    <t>Struct Identifier</t>
-  </si>
-  <si>
     <t>NATYPE</t>
   </si>
   <si>
     <t xml:space="preserve">::= &lt;typeid&gt; def array [ &lt;expr&gt; ] of &lt;structid&gt; end </t>
   </si>
   <si>
-    <t>Array Type Identifier</t>
-  </si>
-  <si>
     <t>NFLIST</t>
   </si>
   <si>
@@ -263,16 +251,10 @@
     <t xml:space="preserve">::= &lt;id&gt; : &lt;stype&gt; </t>
   </si>
   <si>
-    <t>Variable Type</t>
-  </si>
-  <si>
     <t>NTDECL</t>
   </si>
   <si>
     <t xml:space="preserve">::= &lt;id&gt; : &lt;structid&gt; </t>
-  </si>
-  <si>
-    <t>Variable type</t>
   </si>
   <si>
     <t>NALIST</t>
@@ -329,9 +311,6 @@
     <t xml:space="preserve">::= func &lt;id&gt; ( &lt;plist&gt; ) : &lt;rtype&gt; &lt;funcbody&gt; </t>
   </si>
   <si>
-    <t>Function Identifier &amp; return type</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;rtype&gt; </t>
   </si>
   <si>
@@ -374,9 +353,6 @@
     <t xml:space="preserve">::= const &lt;arrdecl&gt; </t>
   </si>
   <si>
-    <t>Apply const to var</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;funcbody&gt; </t>
   </si>
   <si>
@@ -662,7 +638,7 @@
     <t xml:space="preserve">::= &lt;rel&gt; </t>
   </si>
   <si>
-    <t>&lt;boolr&gt; := {Є | &lt;logop&gt; &lt;rel&gt;}</t>
+    <t>&lt;boolr&gt; := {Є | &lt;logop&gt; &lt;rel&gt; &lt;boolr&gt;}</t>
   </si>
   <si>
     <t>NNOT</t>
@@ -761,7 +737,7 @@
     <t xml:space="preserve">::= &lt;expr&gt; - &lt;term&gt; </t>
   </si>
   <si>
-    <t>&lt;exprr&gt; := {+ | -} &lt;term&gt;</t>
+    <t>&lt;exprr&gt; := {+ | -} &lt;term&gt;&lt;exprr&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">::= &lt;term&gt; </t>
@@ -788,7 +764,7 @@
     <t xml:space="preserve">::= &lt;term&gt; / &lt;fact&gt; </t>
   </si>
   <si>
-    <t>&lt;termr&gt; := {* | / | %} &lt;fact&gt;</t>
+    <t>&lt;termr&gt; := {* | / | %} &lt;fact&gt; &lt;termr&gt;</t>
   </si>
   <si>
     <t>NMOD</t>
@@ -818,7 +794,7 @@
     <t xml:space="preserve">::= &lt;exponent&gt; </t>
   </si>
   <si>
-    <t>&lt;factr&gt; := {Є || ^&lt;exponent&gt;}</t>
+    <t>&lt;factr&gt; := {Є || ^&lt;exponent&gt;&lt;factr&gt;}</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;exponent&gt; </t>
@@ -888,7 +864,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1285,25 +1261,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC61397-58B0-444C-B81F-7BA48705ED8A}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:O105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O69" sqref="O69"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:L105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="28.7109375" customWidth="1"/>
     <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1322,22 +1301,20 @@
       <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="2:15">
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1346,21 +1323,16 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4" t="s">
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="2:15">
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -1370,19 +1342,16 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-    </row>
-    <row r="4" spans="2:15">
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -1392,43 +1361,37 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-    </row>
-    <row r="5" spans="2:15">
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="2:15">
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1438,19 +1401,16 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" spans="2:15">
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -1460,21 +1420,16 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15">
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -1484,19 +1439,16 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-    </row>
-    <row r="9" spans="2:15">
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1506,19 +1458,16 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="2:15">
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -1528,19 +1477,16 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="2:15">
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -1550,19 +1496,16 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-    </row>
-    <row r="12" spans="2:15">
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -1572,45 +1515,37 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15">
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-    </row>
-    <row r="14" spans="2:15">
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1620,43 +1555,37 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-    </row>
-    <row r="15" spans="2:15">
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-    </row>
-    <row r="16" spans="2:15">
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1666,19 +1595,16 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-    </row>
-    <row r="17" spans="2:15">
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1688,21 +1614,16 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15">
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1712,21 +1633,16 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15">
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1736,19 +1652,16 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="2:15">
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1758,19 +1671,16 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="2:15">
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -1780,21 +1690,16 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15">
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1804,45 +1709,37 @@
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15">
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-    </row>
-    <row r="24" spans="2:15">
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -1852,19 +1749,16 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-    </row>
-    <row r="25" spans="2:15">
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -1874,21 +1768,16 @@
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15">
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -1898,21 +1787,16 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15">
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -1922,19 +1806,16 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-    </row>
-    <row r="28" spans="2:15">
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -1944,43 +1825,37 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-    </row>
-    <row r="29" spans="2:15">
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-    </row>
-    <row r="30" spans="2:15">
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -1990,19 +1865,16 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-    </row>
-    <row r="31" spans="2:15">
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -2012,19 +1884,16 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-    </row>
-    <row r="32" spans="2:15">
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -2034,19 +1903,16 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-    </row>
-    <row r="33" spans="2:15">
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -2056,21 +1922,16 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="2:15">
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -2080,19 +1941,16 @@
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
-    </row>
-    <row r="35" spans="2:15">
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -2102,43 +1960,37 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-    </row>
-    <row r="36" spans="2:15" ht="15">
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-    </row>
-    <row r="37" spans="2:15">
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -2148,19 +2000,16 @@
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-    </row>
-    <row r="38" spans="2:15">
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -2170,19 +2019,16 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-    </row>
-    <row r="39" spans="2:15">
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -2192,67 +2038,58 @@
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-    </row>
-    <row r="40" spans="2:15">
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-    </row>
-    <row r="41" spans="2:15">
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-    </row>
-    <row r="42" spans="2:15">
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -2262,19 +2099,16 @@
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5"/>
-    </row>
-    <row r="43" spans="2:15">
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -2284,19 +2118,16 @@
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-    </row>
-    <row r="44" spans="2:15">
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -2306,19 +2137,16 @@
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-    </row>
-    <row r="45" spans="2:15">
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -2328,19 +2156,16 @@
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
-    </row>
-    <row r="46" spans="2:15">
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -2350,19 +2175,16 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-    </row>
-    <row r="47" spans="2:15">
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -2372,43 +2194,37 @@
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
-    </row>
-    <row r="48" spans="2:15" ht="15">
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-    </row>
-    <row r="49" spans="2:15" ht="15">
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
@@ -2418,19 +2234,16 @@
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-    </row>
-    <row r="50" spans="2:15">
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -2440,19 +2253,16 @@
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5"/>
-    </row>
-    <row r="51" spans="2:15">
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
@@ -2462,19 +2272,16 @@
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5"/>
-    </row>
-    <row r="52" spans="2:15">
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
@@ -2484,19 +2291,16 @@
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-    </row>
-    <row r="53" spans="2:15">
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
@@ -2506,19 +2310,16 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
-    </row>
-    <row r="54" spans="2:15">
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
@@ -2528,19 +2329,16 @@
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-      <c r="O54" s="5"/>
-    </row>
-    <row r="55" spans="2:15">
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
@@ -2550,19 +2348,16 @@
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
-      <c r="N55" s="5"/>
-      <c r="O55" s="5"/>
-    </row>
-    <row r="56" spans="2:15">
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
@@ -2572,19 +2367,16 @@
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
-      <c r="M56" s="5"/>
-      <c r="N56" s="5"/>
-      <c r="O56" s="5"/>
-    </row>
-    <row r="57" spans="2:15">
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
@@ -2594,19 +2386,16 @@
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
-      <c r="M57" s="5"/>
-      <c r="N57" s="5"/>
-      <c r="O57" s="5"/>
-    </row>
-    <row r="58" spans="2:15">
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C58" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>148</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
@@ -2616,19 +2405,16 @@
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
-      <c r="M58" s="5"/>
-      <c r="N58" s="5"/>
-      <c r="O58" s="5"/>
-    </row>
-    <row r="59" spans="2:15">
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -2638,19 +2424,16 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
-    </row>
-    <row r="60" spans="2:15">
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
@@ -2660,19 +2443,16 @@
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
-      <c r="O60" s="4"/>
-    </row>
-    <row r="61" spans="2:15">
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
@@ -2682,19 +2462,16 @@
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
-    </row>
-    <row r="62" spans="2:15">
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -2704,19 +2481,16 @@
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
-      <c r="M62" s="5"/>
-      <c r="N62" s="5"/>
-      <c r="O62" s="5"/>
-    </row>
-    <row r="63" spans="2:15">
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
@@ -2726,43 +2500,37 @@
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
-    </row>
-    <row r="64" spans="2:15">
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5"/>
-      <c r="O64" s="5"/>
-    </row>
-    <row r="65" spans="2:15">
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
@@ -2772,69 +2540,60 @@
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
-      <c r="M65" s="5"/>
-      <c r="N65" s="5"/>
-      <c r="O65" s="5"/>
-    </row>
-    <row r="66" spans="2:15">
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
       <c r="H66" s="8"/>
       <c r="I66" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
-      <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
-    </row>
-    <row r="67" spans="2:15">
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
       <c r="I67" s="4" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
-      <c r="M67" s="4"/>
-      <c r="N67" s="4"/>
-      <c r="O67" s="4"/>
-    </row>
-    <row r="68" spans="2:15">
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
@@ -2844,43 +2603,37 @@
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
       <c r="L68" s="4"/>
-      <c r="M68" s="4"/>
-      <c r="N68" s="4"/>
-      <c r="O68" s="4"/>
-    </row>
-    <row r="69" spans="2:15">
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5"/>
-      <c r="O69" s="5"/>
-    </row>
-    <row r="70" spans="2:15">
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
@@ -2890,19 +2643,16 @@
       <c r="J70" s="5"/>
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
-      <c r="M70" s="5"/>
-      <c r="N70" s="5"/>
-      <c r="O70" s="5"/>
-    </row>
-    <row r="71" spans="2:15">
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
@@ -2912,21 +2662,18 @@
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
       <c r="L71" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="M71" s="4"/>
-      <c r="N71" s="4"/>
-      <c r="O71" s="4"/>
-    </row>
-    <row r="72" spans="2:15">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
@@ -2936,45 +2683,39 @@
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
       <c r="L72" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="M72" s="4"/>
-      <c r="N72" s="4"/>
-      <c r="O72" s="4"/>
-    </row>
-    <row r="73" spans="2:15">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
+      <c r="I73" s="5" t="s">
+        <v>182</v>
+      </c>
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
-      <c r="L73" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="M73" s="5"/>
-      <c r="N73" s="5"/>
-      <c r="O73" s="5"/>
-    </row>
-    <row r="74" spans="2:15">
+      <c r="L73" s="5"/>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
@@ -2984,19 +2725,16 @@
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
-      <c r="M74" s="5"/>
-      <c r="N74" s="5"/>
-      <c r="O74" s="5"/>
-    </row>
-    <row r="75" spans="2:15">
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
@@ -3006,19 +2744,16 @@
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
-      <c r="M75" s="5"/>
-      <c r="N75" s="5"/>
-      <c r="O75" s="5"/>
-    </row>
-    <row r="76" spans="2:15">
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
@@ -3028,19 +2763,16 @@
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
-      <c r="M76" s="4"/>
-      <c r="N76" s="4"/>
-      <c r="O76" s="4"/>
-    </row>
-    <row r="77" spans="2:15">
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
@@ -3050,19 +2782,16 @@
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
       <c r="L77" s="4"/>
-      <c r="M77" s="4"/>
-      <c r="N77" s="4"/>
-      <c r="O77" s="4"/>
-    </row>
-    <row r="78" spans="2:15">
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -3072,19 +2801,16 @@
       <c r="J78" s="4"/>
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
-      <c r="M78" s="4"/>
-      <c r="N78" s="4"/>
-      <c r="O78" s="4"/>
-    </row>
-    <row r="79" spans="2:15">
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
@@ -3094,19 +2820,16 @@
       <c r="J79" s="5"/>
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
-      <c r="M79" s="5"/>
-      <c r="N79" s="5"/>
-      <c r="O79" s="5"/>
-    </row>
-    <row r="80" spans="2:15">
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
@@ -3116,19 +2839,16 @@
       <c r="J80" s="5"/>
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
-      <c r="M80" s="5"/>
-      <c r="N80" s="5"/>
-      <c r="O80" s="5"/>
-    </row>
-    <row r="81" spans="2:15">
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
@@ -3138,19 +2858,16 @@
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
-      <c r="M81" s="5"/>
-      <c r="N81" s="5"/>
-      <c r="O81" s="5"/>
-    </row>
-    <row r="82" spans="2:15">
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
@@ -3160,19 +2877,16 @@
       <c r="J82" s="5"/>
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
-      <c r="M82" s="5"/>
-      <c r="N82" s="5"/>
-      <c r="O82" s="5"/>
-    </row>
-    <row r="83" spans="2:15">
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C83" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>211</v>
       </c>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
@@ -3182,19 +2896,16 @@
       <c r="J83" s="5"/>
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
-      <c r="M83" s="5"/>
-      <c r="N83" s="5"/>
-      <c r="O83" s="5"/>
-    </row>
-    <row r="84" spans="2:15">
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
@@ -3204,19 +2915,16 @@
       <c r="J84" s="5"/>
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
-      <c r="M84" s="5"/>
-      <c r="N84" s="5"/>
-      <c r="O84" s="5"/>
-    </row>
-    <row r="85" spans="2:15">
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
@@ -3226,21 +2934,18 @@
       <c r="J85" s="4"/>
       <c r="K85" s="4"/>
       <c r="L85" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="M85" s="4"/>
-      <c r="N85" s="4"/>
-      <c r="O85" s="4"/>
-    </row>
-    <row r="86" spans="2:15">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
@@ -3250,21 +2955,18 @@
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
       <c r="L86" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="M86" s="4"/>
-      <c r="N86" s="4"/>
-      <c r="O86" s="4"/>
-    </row>
-    <row r="87" spans="2:15">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
@@ -3274,21 +2976,18 @@
       <c r="J87" s="4"/>
       <c r="K87" s="4"/>
       <c r="L87" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="M87" s="4"/>
-      <c r="N87" s="4"/>
-      <c r="O87" s="4"/>
-    </row>
-    <row r="88" spans="2:15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
@@ -3298,21 +2997,18 @@
       <c r="J88" s="5"/>
       <c r="K88" s="5"/>
       <c r="L88" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="M88" s="5"/>
-      <c r="N88" s="5"/>
-      <c r="O88" s="5"/>
-    </row>
-    <row r="89" spans="2:15">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
@@ -3322,21 +3018,18 @@
       <c r="J89" s="5"/>
       <c r="K89" s="5"/>
       <c r="L89" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="M89" s="5"/>
-      <c r="N89" s="5"/>
-      <c r="O89" s="5"/>
-    </row>
-    <row r="90" spans="2:15">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
@@ -3346,21 +3039,18 @@
       <c r="J90" s="5"/>
       <c r="K90" s="5"/>
       <c r="L90" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="M90" s="5"/>
-      <c r="N90" s="5"/>
-      <c r="O90" s="5"/>
-    </row>
-    <row r="91" spans="2:15">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C91" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="D91" s="5" t="s">
         <v>224</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>233</v>
       </c>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
@@ -3370,19 +3060,16 @@
       <c r="J91" s="5"/>
       <c r="K91" s="5"/>
       <c r="L91" s="5"/>
-      <c r="M91" s="5"/>
-      <c r="N91" s="5"/>
-      <c r="O91" s="5"/>
-    </row>
-    <row r="92" spans="2:15">
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
@@ -3392,21 +3079,18 @@
       <c r="J92" s="4"/>
       <c r="K92" s="4"/>
       <c r="L92" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="M92" s="4"/>
-      <c r="N92" s="4"/>
-      <c r="O92" s="4"/>
-    </row>
-    <row r="93" spans="2:15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
@@ -3416,21 +3100,18 @@
       <c r="J93" s="4"/>
       <c r="K93" s="4"/>
       <c r="L93" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="M93" s="4"/>
-      <c r="N93" s="4"/>
-      <c r="O93" s="4"/>
-    </row>
-    <row r="94" spans="2:15">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
@@ -3440,19 +3121,16 @@
       <c r="J94" s="5"/>
       <c r="K94" s="5"/>
       <c r="L94" s="5"/>
-      <c r="M94" s="5"/>
-      <c r="N94" s="5"/>
-      <c r="O94" s="5"/>
-    </row>
-    <row r="95" spans="2:15">
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
@@ -3462,19 +3140,16 @@
       <c r="J95" s="5"/>
       <c r="K95" s="5"/>
       <c r="L95" s="5"/>
-      <c r="M95" s="5"/>
-      <c r="N95" s="5"/>
-      <c r="O95" s="5"/>
-    </row>
-    <row r="96" spans="2:15">
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
@@ -3484,19 +3159,16 @@
       <c r="J96" s="5"/>
       <c r="K96" s="5"/>
       <c r="L96" s="5"/>
-      <c r="M96" s="5"/>
-      <c r="N96" s="5"/>
-      <c r="O96" s="5"/>
-    </row>
-    <row r="97" spans="2:15">
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="E97" s="5"/>
       <c r="F97" s="5"/>
@@ -3506,19 +3178,16 @@
       <c r="J97" s="5"/>
       <c r="K97" s="5"/>
       <c r="L97" s="5"/>
-      <c r="M97" s="5"/>
-      <c r="N97" s="5"/>
-      <c r="O97" s="5"/>
-    </row>
-    <row r="98" spans="2:15">
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
@@ -3528,19 +3197,16 @@
       <c r="J98" s="5"/>
       <c r="K98" s="5"/>
       <c r="L98" s="5"/>
-      <c r="M98" s="5"/>
-      <c r="N98" s="5"/>
-      <c r="O98" s="5"/>
-    </row>
-    <row r="99" spans="2:15">
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C99" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D99" s="5" t="s">
         <v>240</v>
-      </c>
-      <c r="D99" s="5" t="s">
-        <v>249</v>
       </c>
       <c r="E99" s="5"/>
       <c r="F99" s="5"/>
@@ -3550,19 +3216,16 @@
       <c r="J99" s="5"/>
       <c r="K99" s="5"/>
       <c r="L99" s="5"/>
-      <c r="M99" s="5"/>
-      <c r="N99" s="5"/>
-      <c r="O99" s="5"/>
-    </row>
-    <row r="100" spans="2:15">
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="E100" s="5"/>
       <c r="F100" s="5"/>
@@ -3572,19 +3235,16 @@
       <c r="J100" s="5"/>
       <c r="K100" s="5"/>
       <c r="L100" s="5"/>
-      <c r="M100" s="5"/>
-      <c r="N100" s="5"/>
-      <c r="O100" s="5"/>
-    </row>
-    <row r="101" spans="2:15">
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
@@ -3594,43 +3254,37 @@
       <c r="J101" s="4"/>
       <c r="K101" s="4"/>
       <c r="L101" s="4"/>
-      <c r="M101" s="4"/>
-      <c r="N101" s="4"/>
-      <c r="O101" s="4"/>
-    </row>
-    <row r="102" spans="2:15" ht="15">
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
       <c r="H102" s="5"/>
       <c r="I102" s="5" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="J102" s="5"/>
       <c r="K102" s="5"/>
       <c r="L102" s="5"/>
-      <c r="M102" s="5"/>
-      <c r="N102" s="5"/>
-      <c r="O102" s="5"/>
-    </row>
-    <row r="103" spans="2:15">
+    </row>
+    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="E103" s="5"/>
       <c r="F103" s="5"/>
@@ -3640,19 +3294,16 @@
       <c r="J103" s="5"/>
       <c r="K103" s="5"/>
       <c r="L103" s="5"/>
-      <c r="M103" s="5"/>
-      <c r="N103" s="5"/>
-      <c r="O103" s="5"/>
-    </row>
-    <row r="104" spans="2:15">
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
@@ -3662,19 +3313,16 @@
       <c r="J104" s="4"/>
       <c r="K104" s="4"/>
       <c r="L104" s="4"/>
-      <c r="M104" s="4"/>
-      <c r="N104" s="4"/>
-      <c r="O104" s="4"/>
-    </row>
-    <row r="105" spans="2:15">
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
@@ -3684,15 +3332,12 @@
       <c r="J105" s="4"/>
       <c r="K105" s="4"/>
       <c r="L105" s="4"/>
-      <c r="M105" s="4"/>
-      <c r="N105" s="4"/>
-      <c r="O105" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E66:H68"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" scale="95" fitToWidth="2" fitToHeight="2" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add updated grammar conversion spreadsheet (#14)
</commit_message>
<xml_diff>
--- a/source_language_spec/Grammar_Conversion.xlsx
+++ b/source_language_spec/Grammar_Conversion.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d42660897f176d1e/Documents/Uni/2022/Semester 2/COMP3290/Assessment/Assignment 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A55B4F5E-CA0E-4ACA-B9A2-3FA6FE79AEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="344" documentId="8_{4B6A1E2B-9DE3-4CEB-8A4E-7724E9331625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08EE5BEE-A678-4F03-8B38-AC2B5220AC6A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{CAC1321C-A57E-482A-BF8B-9CDDCA90FB4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAC1321C-A57E-482A-BF8B-9CDDCA90FB4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet2!$B$1:$O$105</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="252">
   <si>
     <t>Node</t>
   </si>
@@ -56,9 +59,6 @@
     <t>Left Recursion</t>
   </si>
   <si>
-    <t>Symbol Table Entry</t>
-  </si>
-  <si>
     <t>NPROG</t>
   </si>
   <si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>CD22, ID done globals started</t>
-  </si>
-  <si>
-    <t>Program Identifier</t>
   </si>
   <si>
     <t>NGLOB</t>
@@ -137,9 +134,6 @@
     <t xml:space="preserve">::= &lt;id&gt; = &lt;expr&gt; </t>
   </si>
   <si>
-    <t>Constant Value</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;types&gt; </t>
   </si>
   <si>
@@ -233,18 +227,12 @@
     <t xml:space="preserve">::= &lt;structid&gt; def &lt;fields&gt; end </t>
   </si>
   <si>
-    <t>Struct Identifier</t>
-  </si>
-  <si>
     <t>NATYPE</t>
   </si>
   <si>
     <t xml:space="preserve">::= &lt;typeid&gt; def array [ &lt;expr&gt; ] of &lt;structid&gt; end </t>
   </si>
   <si>
-    <t>Array Type Identifier</t>
-  </si>
-  <si>
     <t>NFLIST</t>
   </si>
   <si>
@@ -263,16 +251,10 @@
     <t xml:space="preserve">::= &lt;id&gt; : &lt;stype&gt; </t>
   </si>
   <si>
-    <t>Variable Type</t>
-  </si>
-  <si>
     <t>NTDECL</t>
   </si>
   <si>
     <t xml:space="preserve">::= &lt;id&gt; : &lt;structid&gt; </t>
-  </si>
-  <si>
-    <t>Variable type</t>
   </si>
   <si>
     <t>NALIST</t>
@@ -329,9 +311,6 @@
     <t xml:space="preserve">::= func &lt;id&gt; ( &lt;plist&gt; ) : &lt;rtype&gt; &lt;funcbody&gt; </t>
   </si>
   <si>
-    <t>Function Identifier &amp; return type</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;rtype&gt; </t>
   </si>
   <si>
@@ -374,9 +353,6 @@
     <t xml:space="preserve">::= const &lt;arrdecl&gt; </t>
   </si>
   <si>
-    <t>Apply const to var</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;funcbody&gt; </t>
   </si>
   <si>
@@ -662,7 +638,7 @@
     <t xml:space="preserve">::= &lt;rel&gt; </t>
   </si>
   <si>
-    <t>&lt;boolr&gt; := {Є | &lt;logop&gt; &lt;rel&gt;}</t>
+    <t>&lt;boolr&gt; := {Є | &lt;logop&gt; &lt;rel&gt; &lt;boolr&gt;}</t>
   </si>
   <si>
     <t>NNOT</t>
@@ -761,7 +737,7 @@
     <t xml:space="preserve">::= &lt;expr&gt; - &lt;term&gt; </t>
   </si>
   <si>
-    <t>&lt;exprr&gt; := {+ | -} &lt;term&gt;</t>
+    <t>&lt;exprr&gt; := {+ | -} &lt;term&gt;&lt;exprr&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">::= &lt;term&gt; </t>
@@ -788,7 +764,7 @@
     <t xml:space="preserve">::= &lt;term&gt; / &lt;fact&gt; </t>
   </si>
   <si>
-    <t>&lt;termr&gt; := {* | / | %} &lt;fact&gt;</t>
+    <t>&lt;termr&gt; := {* | / | %} &lt;fact&gt; &lt;termr&gt;</t>
   </si>
   <si>
     <t>NMOD</t>
@@ -818,7 +794,7 @@
     <t xml:space="preserve">::= &lt;exponent&gt; </t>
   </si>
   <si>
-    <t>&lt;factr&gt; := {Є || ^&lt;exponent&gt;}</t>
+    <t>&lt;factr&gt; := {Є || ^&lt;exponent&gt;&lt;factr&gt;}</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;exponent&gt; </t>
@@ -888,7 +864,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1285,25 +1261,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC61397-58B0-444C-B81F-7BA48705ED8A}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:O105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O69" sqref="O69"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:L105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="28.7109375" customWidth="1"/>
     <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1322,22 +1301,20 @@
       <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="2:15">
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1346,21 +1323,16 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4" t="s">
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="2:15">
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -1370,19 +1342,16 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-    </row>
-    <row r="4" spans="2:15">
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -1392,43 +1361,37 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-    </row>
-    <row r="5" spans="2:15">
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="2:15">
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1438,19 +1401,16 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" spans="2:15">
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -1460,21 +1420,16 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15">
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -1484,19 +1439,16 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-    </row>
-    <row r="9" spans="2:15">
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1506,19 +1458,16 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="2:15">
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -1528,19 +1477,16 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="2:15">
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -1550,19 +1496,16 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-    </row>
-    <row r="12" spans="2:15">
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -1572,45 +1515,37 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15">
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-    </row>
-    <row r="14" spans="2:15">
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1620,43 +1555,37 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-    </row>
-    <row r="15" spans="2:15">
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-    </row>
-    <row r="16" spans="2:15">
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1666,19 +1595,16 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-    </row>
-    <row r="17" spans="2:15">
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1688,21 +1614,16 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15">
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1712,21 +1633,16 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15">
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1736,19 +1652,16 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="2:15">
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1758,19 +1671,16 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="2:15">
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -1780,21 +1690,16 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15">
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1804,45 +1709,37 @@
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15">
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-    </row>
-    <row r="24" spans="2:15">
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -1852,19 +1749,16 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-    </row>
-    <row r="25" spans="2:15">
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -1874,21 +1768,16 @@
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15">
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -1898,21 +1787,16 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15">
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -1922,19 +1806,16 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-    </row>
-    <row r="28" spans="2:15">
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -1944,43 +1825,37 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-    </row>
-    <row r="29" spans="2:15">
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-    </row>
-    <row r="30" spans="2:15">
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -1990,19 +1865,16 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-    </row>
-    <row r="31" spans="2:15">
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -2012,19 +1884,16 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-    </row>
-    <row r="32" spans="2:15">
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -2034,19 +1903,16 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-    </row>
-    <row r="33" spans="2:15">
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -2056,21 +1922,16 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="2:15">
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -2080,19 +1941,16 @@
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
-    </row>
-    <row r="35" spans="2:15">
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -2102,43 +1960,37 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-    </row>
-    <row r="36" spans="2:15" ht="15">
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-    </row>
-    <row r="37" spans="2:15">
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -2148,19 +2000,16 @@
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-    </row>
-    <row r="38" spans="2:15">
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -2170,19 +2019,16 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-    </row>
-    <row r="39" spans="2:15">
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -2192,67 +2038,58 @@
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-    </row>
-    <row r="40" spans="2:15">
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-    </row>
-    <row r="41" spans="2:15">
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-    </row>
-    <row r="42" spans="2:15">
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -2262,19 +2099,16 @@
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5"/>
-    </row>
-    <row r="43" spans="2:15">
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -2284,19 +2118,16 @@
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-    </row>
-    <row r="44" spans="2:15">
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -2306,19 +2137,16 @@
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-    </row>
-    <row r="45" spans="2:15">
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -2328,19 +2156,16 @@
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
-    </row>
-    <row r="46" spans="2:15">
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -2350,19 +2175,16 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-    </row>
-    <row r="47" spans="2:15">
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -2372,43 +2194,37 @@
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
-    </row>
-    <row r="48" spans="2:15" ht="15">
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-    </row>
-    <row r="49" spans="2:15" ht="15">
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
@@ -2418,19 +2234,16 @@
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-    </row>
-    <row r="50" spans="2:15">
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -2440,19 +2253,16 @@
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5"/>
-    </row>
-    <row r="51" spans="2:15">
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
@@ -2462,19 +2272,16 @@
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5"/>
-    </row>
-    <row r="52" spans="2:15">
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
@@ -2484,19 +2291,16 @@
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-    </row>
-    <row r="53" spans="2:15">
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
@@ -2506,19 +2310,16 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
-    </row>
-    <row r="54" spans="2:15">
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
@@ -2528,19 +2329,16 @@
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-      <c r="O54" s="5"/>
-    </row>
-    <row r="55" spans="2:15">
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
@@ -2550,19 +2348,16 @@
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
-      <c r="N55" s="5"/>
-      <c r="O55" s="5"/>
-    </row>
-    <row r="56" spans="2:15">
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
@@ -2572,19 +2367,16 @@
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
-      <c r="M56" s="5"/>
-      <c r="N56" s="5"/>
-      <c r="O56" s="5"/>
-    </row>
-    <row r="57" spans="2:15">
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
@@ -2594,19 +2386,16 @@
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
-      <c r="M57" s="5"/>
-      <c r="N57" s="5"/>
-      <c r="O57" s="5"/>
-    </row>
-    <row r="58" spans="2:15">
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C58" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>148</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
@@ -2616,19 +2405,16 @@
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
-      <c r="M58" s="5"/>
-      <c r="N58" s="5"/>
-      <c r="O58" s="5"/>
-    </row>
-    <row r="59" spans="2:15">
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -2638,19 +2424,16 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
-    </row>
-    <row r="60" spans="2:15">
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
@@ -2660,19 +2443,16 @@
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
-      <c r="O60" s="4"/>
-    </row>
-    <row r="61" spans="2:15">
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
@@ -2682,19 +2462,16 @@
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
-    </row>
-    <row r="62" spans="2:15">
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -2704,19 +2481,16 @@
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
-      <c r="M62" s="5"/>
-      <c r="N62" s="5"/>
-      <c r="O62" s="5"/>
-    </row>
-    <row r="63" spans="2:15">
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
@@ -2726,43 +2500,37 @@
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
-    </row>
-    <row r="64" spans="2:15">
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5"/>
-      <c r="O64" s="5"/>
-    </row>
-    <row r="65" spans="2:15">
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
@@ -2772,69 +2540,60 @@
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
-      <c r="M65" s="5"/>
-      <c r="N65" s="5"/>
-      <c r="O65" s="5"/>
-    </row>
-    <row r="66" spans="2:15">
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
       <c r="H66" s="8"/>
       <c r="I66" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
-      <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
-    </row>
-    <row r="67" spans="2:15">
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
       <c r="I67" s="4" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
-      <c r="M67" s="4"/>
-      <c r="N67" s="4"/>
-      <c r="O67" s="4"/>
-    </row>
-    <row r="68" spans="2:15">
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
@@ -2844,43 +2603,37 @@
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
       <c r="L68" s="4"/>
-      <c r="M68" s="4"/>
-      <c r="N68" s="4"/>
-      <c r="O68" s="4"/>
-    </row>
-    <row r="69" spans="2:15">
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5"/>
-      <c r="O69" s="5"/>
-    </row>
-    <row r="70" spans="2:15">
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
@@ -2890,19 +2643,16 @@
       <c r="J70" s="5"/>
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
-      <c r="M70" s="5"/>
-      <c r="N70" s="5"/>
-      <c r="O70" s="5"/>
-    </row>
-    <row r="71" spans="2:15">
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
@@ -2912,21 +2662,18 @@
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
       <c r="L71" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="M71" s="4"/>
-      <c r="N71" s="4"/>
-      <c r="O71" s="4"/>
-    </row>
-    <row r="72" spans="2:15">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
@@ -2936,45 +2683,39 @@
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
       <c r="L72" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="M72" s="4"/>
-      <c r="N72" s="4"/>
-      <c r="O72" s="4"/>
-    </row>
-    <row r="73" spans="2:15">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
+      <c r="I73" s="5" t="s">
+        <v>182</v>
+      </c>
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
-      <c r="L73" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="M73" s="5"/>
-      <c r="N73" s="5"/>
-      <c r="O73" s="5"/>
-    </row>
-    <row r="74" spans="2:15">
+      <c r="L73" s="5"/>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
@@ -2984,19 +2725,16 @@
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
-      <c r="M74" s="5"/>
-      <c r="N74" s="5"/>
-      <c r="O74" s="5"/>
-    </row>
-    <row r="75" spans="2:15">
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
@@ -3006,19 +2744,16 @@
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
-      <c r="M75" s="5"/>
-      <c r="N75" s="5"/>
-      <c r="O75" s="5"/>
-    </row>
-    <row r="76" spans="2:15">
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
@@ -3028,19 +2763,16 @@
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
-      <c r="M76" s="4"/>
-      <c r="N76" s="4"/>
-      <c r="O76" s="4"/>
-    </row>
-    <row r="77" spans="2:15">
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
@@ -3050,19 +2782,16 @@
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
       <c r="L77" s="4"/>
-      <c r="M77" s="4"/>
-      <c r="N77" s="4"/>
-      <c r="O77" s="4"/>
-    </row>
-    <row r="78" spans="2:15">
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -3072,19 +2801,16 @@
       <c r="J78" s="4"/>
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
-      <c r="M78" s="4"/>
-      <c r="N78" s="4"/>
-      <c r="O78" s="4"/>
-    </row>
-    <row r="79" spans="2:15">
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
@@ -3094,19 +2820,16 @@
       <c r="J79" s="5"/>
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
-      <c r="M79" s="5"/>
-      <c r="N79" s="5"/>
-      <c r="O79" s="5"/>
-    </row>
-    <row r="80" spans="2:15">
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
@@ -3116,19 +2839,16 @@
       <c r="J80" s="5"/>
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
-      <c r="M80" s="5"/>
-      <c r="N80" s="5"/>
-      <c r="O80" s="5"/>
-    </row>
-    <row r="81" spans="2:15">
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
@@ -3138,19 +2858,16 @@
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
-      <c r="M81" s="5"/>
-      <c r="N81" s="5"/>
-      <c r="O81" s="5"/>
-    </row>
-    <row r="82" spans="2:15">
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
@@ -3160,19 +2877,16 @@
       <c r="J82" s="5"/>
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
-      <c r="M82" s="5"/>
-      <c r="N82" s="5"/>
-      <c r="O82" s="5"/>
-    </row>
-    <row r="83" spans="2:15">
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C83" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>211</v>
       </c>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
@@ -3182,19 +2896,16 @@
       <c r="J83" s="5"/>
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
-      <c r="M83" s="5"/>
-      <c r="N83" s="5"/>
-      <c r="O83" s="5"/>
-    </row>
-    <row r="84" spans="2:15">
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
@@ -3204,19 +2915,16 @@
       <c r="J84" s="5"/>
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
-      <c r="M84" s="5"/>
-      <c r="N84" s="5"/>
-      <c r="O84" s="5"/>
-    </row>
-    <row r="85" spans="2:15">
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
@@ -3226,21 +2934,18 @@
       <c r="J85" s="4"/>
       <c r="K85" s="4"/>
       <c r="L85" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="M85" s="4"/>
-      <c r="N85" s="4"/>
-      <c r="O85" s="4"/>
-    </row>
-    <row r="86" spans="2:15">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
@@ -3250,21 +2955,18 @@
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
       <c r="L86" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="M86" s="4"/>
-      <c r="N86" s="4"/>
-      <c r="O86" s="4"/>
-    </row>
-    <row r="87" spans="2:15">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
@@ -3274,21 +2976,18 @@
       <c r="J87" s="4"/>
       <c r="K87" s="4"/>
       <c r="L87" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="M87" s="4"/>
-      <c r="N87" s="4"/>
-      <c r="O87" s="4"/>
-    </row>
-    <row r="88" spans="2:15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
@@ -3298,21 +2997,18 @@
       <c r="J88" s="5"/>
       <c r="K88" s="5"/>
       <c r="L88" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="M88" s="5"/>
-      <c r="N88" s="5"/>
-      <c r="O88" s="5"/>
-    </row>
-    <row r="89" spans="2:15">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
@@ -3322,21 +3018,18 @@
       <c r="J89" s="5"/>
       <c r="K89" s="5"/>
       <c r="L89" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="M89" s="5"/>
-      <c r="N89" s="5"/>
-      <c r="O89" s="5"/>
-    </row>
-    <row r="90" spans="2:15">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
@@ -3346,21 +3039,18 @@
       <c r="J90" s="5"/>
       <c r="K90" s="5"/>
       <c r="L90" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="M90" s="5"/>
-      <c r="N90" s="5"/>
-      <c r="O90" s="5"/>
-    </row>
-    <row r="91" spans="2:15">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C91" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="D91" s="5" t="s">
         <v>224</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>233</v>
       </c>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
@@ -3370,19 +3060,16 @@
       <c r="J91" s="5"/>
       <c r="K91" s="5"/>
       <c r="L91" s="5"/>
-      <c r="M91" s="5"/>
-      <c r="N91" s="5"/>
-      <c r="O91" s="5"/>
-    </row>
-    <row r="92" spans="2:15">
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
@@ -3392,21 +3079,18 @@
       <c r="J92" s="4"/>
       <c r="K92" s="4"/>
       <c r="L92" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="M92" s="4"/>
-      <c r="N92" s="4"/>
-      <c r="O92" s="4"/>
-    </row>
-    <row r="93" spans="2:15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
@@ -3416,21 +3100,18 @@
       <c r="J93" s="4"/>
       <c r="K93" s="4"/>
       <c r="L93" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="M93" s="4"/>
-      <c r="N93" s="4"/>
-      <c r="O93" s="4"/>
-    </row>
-    <row r="94" spans="2:15">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
@@ -3440,19 +3121,16 @@
       <c r="J94" s="5"/>
       <c r="K94" s="5"/>
       <c r="L94" s="5"/>
-      <c r="M94" s="5"/>
-      <c r="N94" s="5"/>
-      <c r="O94" s="5"/>
-    </row>
-    <row r="95" spans="2:15">
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
@@ -3462,19 +3140,16 @@
       <c r="J95" s="5"/>
       <c r="K95" s="5"/>
       <c r="L95" s="5"/>
-      <c r="M95" s="5"/>
-      <c r="N95" s="5"/>
-      <c r="O95" s="5"/>
-    </row>
-    <row r="96" spans="2:15">
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
@@ -3484,19 +3159,16 @@
       <c r="J96" s="5"/>
       <c r="K96" s="5"/>
       <c r="L96" s="5"/>
-      <c r="M96" s="5"/>
-      <c r="N96" s="5"/>
-      <c r="O96" s="5"/>
-    </row>
-    <row r="97" spans="2:15">
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="E97" s="5"/>
       <c r="F97" s="5"/>
@@ -3506,19 +3178,16 @@
       <c r="J97" s="5"/>
       <c r="K97" s="5"/>
       <c r="L97" s="5"/>
-      <c r="M97" s="5"/>
-      <c r="N97" s="5"/>
-      <c r="O97" s="5"/>
-    </row>
-    <row r="98" spans="2:15">
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
@@ -3528,19 +3197,16 @@
       <c r="J98" s="5"/>
       <c r="K98" s="5"/>
       <c r="L98" s="5"/>
-      <c r="M98" s="5"/>
-      <c r="N98" s="5"/>
-      <c r="O98" s="5"/>
-    </row>
-    <row r="99" spans="2:15">
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C99" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D99" s="5" t="s">
         <v>240</v>
-      </c>
-      <c r="D99" s="5" t="s">
-        <v>249</v>
       </c>
       <c r="E99" s="5"/>
       <c r="F99" s="5"/>
@@ -3550,19 +3216,16 @@
       <c r="J99" s="5"/>
       <c r="K99" s="5"/>
       <c r="L99" s="5"/>
-      <c r="M99" s="5"/>
-      <c r="N99" s="5"/>
-      <c r="O99" s="5"/>
-    </row>
-    <row r="100" spans="2:15">
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="E100" s="5"/>
       <c r="F100" s="5"/>
@@ -3572,19 +3235,16 @@
       <c r="J100" s="5"/>
       <c r="K100" s="5"/>
       <c r="L100" s="5"/>
-      <c r="M100" s="5"/>
-      <c r="N100" s="5"/>
-      <c r="O100" s="5"/>
-    </row>
-    <row r="101" spans="2:15">
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
@@ -3594,43 +3254,37 @@
       <c r="J101" s="4"/>
       <c r="K101" s="4"/>
       <c r="L101" s="4"/>
-      <c r="M101" s="4"/>
-      <c r="N101" s="4"/>
-      <c r="O101" s="4"/>
-    </row>
-    <row r="102" spans="2:15" ht="15">
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
       <c r="H102" s="5"/>
       <c r="I102" s="5" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="J102" s="5"/>
       <c r="K102" s="5"/>
       <c r="L102" s="5"/>
-      <c r="M102" s="5"/>
-      <c r="N102" s="5"/>
-      <c r="O102" s="5"/>
-    </row>
-    <row r="103" spans="2:15">
+    </row>
+    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="E103" s="5"/>
       <c r="F103" s="5"/>
@@ -3640,19 +3294,16 @@
       <c r="J103" s="5"/>
       <c r="K103" s="5"/>
       <c r="L103" s="5"/>
-      <c r="M103" s="5"/>
-      <c r="N103" s="5"/>
-      <c r="O103" s="5"/>
-    </row>
-    <row r="104" spans="2:15">
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
@@ -3662,19 +3313,16 @@
       <c r="J104" s="4"/>
       <c r="K104" s="4"/>
       <c r="L104" s="4"/>
-      <c r="M104" s="4"/>
-      <c r="N104" s="4"/>
-      <c r="O104" s="4"/>
-    </row>
-    <row r="105" spans="2:15">
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
@@ -3684,15 +3332,12 @@
       <c r="J105" s="4"/>
       <c r="K105" s="4"/>
       <c r="L105" s="4"/>
-      <c r="M105" s="4"/>
-      <c r="N105" s="4"/>
-      <c r="O105" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E66:H68"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" scale="95" fitToWidth="2" fitToHeight="2" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>